<commit_message>
Update census, collection and data file with new requests
</commit_message>
<xml_diff>
--- a/Census_Wsc_Services.xlsx
+++ b/Census_Wsc_Services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F962697D-D9FA-A646-A8BD-1ACB36EC90A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9990427-E6CD-9C45-8AED-769EDC50E5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
+    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="237">
   <si>
     <t>Service Category</t>
   </si>
@@ -733,6 +733,18 @@
   </si>
   <si>
     <t>NOT SUPPORTED ANYMORE</t>
+  </si>
+  <si>
+    <t>utente_automationtest@test.it</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>actually 200</t>
+  </si>
+  <si>
+    <t>To check by QA</t>
   </si>
 </sst>
 </file>
@@ -1307,8 +1319,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU200" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1325,7 +1337,7 @@
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.83203125" style="41" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="5"/>
@@ -1382,14 +1394,14 @@
       <c r="G2" s="17"/>
       <c r="H2" s="10"/>
       <c r="M2" s="18" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>230</v>
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1402,8 +1414,8 @@
       <c r="G3" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>211</v>
+      <c r="M3" s="18" t="s">
+        <v>233</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>231</v>
@@ -1416,7 +1428,7 @@
       <c r="G4" s="11"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>4</v>
       </c>
@@ -1434,9 +1446,12 @@
       <c r="G5" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H5" s="6" t="s">
+        <v>204</v>
+      </c>
       <c r="O5" s="22"/>
     </row>
-    <row r="6" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -1452,9 +1467,12 @@
       <c r="G6" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H6" s="6" t="s">
+        <v>204</v>
+      </c>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -1470,9 +1488,15 @@
       <c r="G7" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H7" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7" s="5">
+        <v>422</v>
+      </c>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -1488,9 +1512,15 @@
       <c r="G8" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H8" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8" s="5">
+        <v>422</v>
+      </c>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -1506,8 +1536,14 @@
       <c r="G9" s="19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="5">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
@@ -1523,8 +1559,14 @@
       <c r="G10" s="19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -1541,7 +1583,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -1558,7 +1600,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -1575,7 +1617,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="40"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
@@ -1592,7 +1634,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -1609,7 +1651,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40"/>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -1626,7 +1668,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
@@ -1643,7 +1685,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="40"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
@@ -1660,7 +1702,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -1921,7 +1963,7 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="40"/>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
@@ -1944,7 +1986,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="40"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -2152,7 +2194,7 @@
       </c>
       <c r="G49" s="12"/>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="40"/>
       <c r="B50" s="40" t="s">
         <v>58</v>
@@ -2171,7 +2213,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="40"/>
       <c r="B51" s="40"/>
       <c r="C51" s="40"/>
@@ -2245,7 +2287,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="40"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
@@ -2260,7 +2302,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="40"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
@@ -2275,7 +2317,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="40"/>
       <c r="B56" s="40" t="s">
         <v>72</v>
@@ -2296,7 +2338,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="40"/>
       <c r="B57" s="40"/>
       <c r="C57" s="40"/>
@@ -2313,7 +2355,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="40"/>
       <c r="B58" s="40"/>
       <c r="C58" s="40"/>
@@ -2330,7 +2372,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="40"/>
       <c r="B59" s="40"/>
       <c r="C59" s="40"/>
@@ -2347,7 +2389,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="40"/>
       <c r="B60" s="40"/>
       <c r="C60" s="40"/>
@@ -2694,7 +2736,7 @@
       <c r="J75" s="37"/>
       <c r="K75" s="36"/>
     </row>
-    <row r="76" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="40"/>
       <c r="B76" s="40"/>
       <c r="C76" s="40"/>
@@ -2720,7 +2762,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="40"/>
       <c r="B77" s="40"/>
       <c r="C77" s="40"/>
@@ -2769,7 +2811,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="40"/>
       <c r="B79" s="40"/>
       <c r="C79" s="40"/>
@@ -2795,7 +2837,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="40"/>
       <c r="B80" s="40"/>
       <c r="C80" s="40"/>
@@ -2862,7 +2904,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="40"/>
       <c r="B83" s="40"/>
       <c r="C83" s="40"/>
@@ -2891,7 +2933,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="40"/>
       <c r="B84" s="40"/>
       <c r="C84" s="40"/>
@@ -2920,7 +2962,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="40"/>
       <c r="B85" s="40"/>
       <c r="C85" s="40"/>
@@ -2949,7 +2991,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="40"/>
       <c r="B86" s="40"/>
       <c r="C86" s="40"/>
@@ -3196,7 +3238,7 @@
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="38" t="s">
         <v>116</v>
       </c>
@@ -3214,8 +3256,14 @@
       <c r="G100" s="21" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H100" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="38"/>
       <c r="B101" s="38"/>
       <c r="C101" s="38"/>
@@ -3231,8 +3279,14 @@
       <c r="G101" s="21" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H101" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
       <c r="C102" s="38"/>
@@ -3248,8 +3302,11 @@
       <c r="G102" s="21" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H102" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="38"/>
       <c r="B103" s="38"/>
       <c r="C103" s="38"/>
@@ -3264,6 +3321,9 @@
       </c>
       <c r="G103" s="21" t="s">
         <v>202</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3416,7 +3476,7 @@
       </c>
       <c r="G113" s="13"/>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="38"/>
       <c r="B114" s="38"/>
       <c r="C114" s="38"/>
@@ -3432,8 +3492,11 @@
       <c r="G114" s="21" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H114" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="38"/>
       <c r="B115" s="38"/>
       <c r="C115" s="38"/>
@@ -3448,6 +3511,9 @@
       </c>
       <c r="G115" s="21" t="s">
         <v>202</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3488,7 +3554,7 @@
     <row r="119" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
     </row>
-    <row r="120" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="40" t="s">
         <v>136</v>
       </c>
@@ -3509,7 +3575,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="40"/>
       <c r="B121" s="38"/>
       <c r="C121" s="38"/>
@@ -3526,7 +3592,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="40"/>
       <c r="B122" s="38"/>
       <c r="C122" s="38"/>
@@ -3543,7 +3609,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="40"/>
       <c r="B123" s="38"/>
       <c r="C123" s="38"/>
@@ -3560,7 +3626,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="40"/>
       <c r="B124" s="38"/>
       <c r="C124" s="38"/>
@@ -3586,7 +3652,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="40"/>
       <c r="B125" s="38"/>
       <c r="C125" s="38"/>
@@ -3606,7 +3672,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="40"/>
       <c r="B126" s="38"/>
       <c r="C126" s="38"/>
@@ -3626,7 +3692,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="40"/>
       <c r="B127" s="38"/>
       <c r="C127" s="38"/>
@@ -3646,7 +3712,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="40"/>
       <c r="B128" s="38"/>
       <c r="C128" s="38"/>
@@ -3666,7 +3732,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="40"/>
       <c r="B129" s="38"/>
       <c r="C129" s="38"/>
@@ -3686,7 +3752,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="40"/>
       <c r="B130" s="38"/>
       <c r="C130" s="38"/>
@@ -3706,7 +3772,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="40"/>
       <c r="B131" s="38"/>
       <c r="C131" s="38"/>
@@ -3726,7 +3792,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="40"/>
       <c r="B132" s="38"/>
       <c r="C132" s="38"/>
@@ -3746,7 +3812,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="40"/>
       <c r="B133" s="38"/>
       <c r="C133" s="38"/>
@@ -3766,7 +3832,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="40"/>
       <c r="B134" s="38"/>
       <c r="C134" s="38"/>
@@ -3786,7 +3852,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="40"/>
       <c r="B135" s="38"/>
       <c r="C135" s="38"/>
@@ -3806,7 +3872,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="40"/>
       <c r="B136" s="38"/>
       <c r="C136" s="38"/>
@@ -3826,7 +3892,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="40"/>
       <c r="B137" s="38"/>
       <c r="C137" s="38"/>
@@ -3846,7 +3912,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="40"/>
       <c r="B138" s="38"/>
       <c r="C138" s="38"/>
@@ -3981,7 +4047,7 @@
     <row r="147" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>165</v>
       </c>
@@ -3998,7 +4064,7 @@
     <row r="149" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
     </row>
-    <row r="150" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="38" t="s">
         <v>167</v>
       </c>
@@ -4017,7 +4083,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="38"/>
       <c r="B151" s="38"/>
       <c r="C151" s="38"/>
@@ -4087,7 +4153,7 @@
     <row r="156" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
     </row>
-    <row r="157" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="38" t="s">
         <v>224</v>
       </c>
@@ -4106,7 +4172,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="38"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -4123,7 +4189,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="38"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -4193,7 +4259,7 @@
     <row r="164" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
     </row>
-    <row r="165" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
         <v>198</v>
       </c>
@@ -4215,7 +4281,7 @@
     <row r="166" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
     </row>
-    <row r="167" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="38" t="s">
         <v>76</v>
       </c>
@@ -4234,7 +4300,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="38"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -4254,7 +4320,7 @@
     <row r="169" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
     </row>
-    <row r="170" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="38" t="s">
         <v>184</v>
       </c>
@@ -4273,7 +4339,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="38"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -4355,7 +4421,7 @@
       </c>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="38"/>
       <c r="B177" s="38"/>
       <c r="C177" s="38"/>
@@ -4370,10 +4436,10 @@
       </c>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
     </row>
-    <row r="179" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>193</v>
       </c>
@@ -4390,10 +4456,10 @@
       </c>
       <c r="G179" s="2"/>
     </row>
-    <row r="180" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
     </row>
-    <row r="181" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="D181" s="18" t="s">
         <v>195</v>
@@ -4405,8 +4471,14 @@
       <c r="G181" s="19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H181" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I181" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="D182" s="18" t="s">
         <v>196</v>
@@ -4418,8 +4490,11 @@
       <c r="G182" s="19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H182" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="D183" s="18" t="s">
         <v>197</v>
@@ -4431,23 +4506,15 @@
       <c r="G183" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H183" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="E1:H183" xr:uid="{9EEAC858-8201-E147-9707-1E1D2225B431}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="BB/TV"/>
-        <filter val="Only TV"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="GET"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="High"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update collection, data and environment file
</commit_message>
<xml_diff>
--- a/Census_Wsc_Services.xlsx
+++ b/Census_Wsc_Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9990427-E6CD-9C45-8AED-769EDC50E5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF82E13-4FFA-1849-8FF7-5558C361CAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="236">
   <si>
     <t>Service Category</t>
   </si>
@@ -654,9 +654,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>DP Needed for test Env.</t>
-  </si>
-  <si>
     <t>BLOCKED</t>
   </si>
   <si>
@@ -744,7 +741,7 @@
     <t>actually 200</t>
   </si>
   <si>
-    <t>To check by QA</t>
+    <t>One shot</t>
   </si>
 </sst>
 </file>
@@ -992,16 +989,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1316,11 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8614AE-DEFA-8446-B769-F8D977213401}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1332,7 @@
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="41" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="38" customWidth="1"/>
     <col min="13" max="13" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -1357,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>22</v>
@@ -1372,32 +1368,32 @@
         <v>205</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="L1" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="O1" s="32"/>
     </row>
-    <row r="2" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="F2" s="10"/>
       <c r="G2" s="17"/>
       <c r="H2" s="10"/>
       <c r="M2" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O2" s="9"/>
     </row>
@@ -1415,30 +1411,30 @@
         <v>200</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>23</v>
@@ -1452,14 +1448,14 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>23</v>
@@ -1473,14 +1469,14 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>23</v>
@@ -1489,22 +1485,19 @@
         <v>200</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I7" s="5">
-        <v>422</v>
+        <v>204</v>
       </c>
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>23</v>
@@ -1513,22 +1506,19 @@
         <v>200</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I8" s="5">
-        <v>422</v>
+        <v>204</v>
       </c>
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>23</v>
@@ -1537,21 +1527,18 @@
         <v>200</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" s="5">
-        <v>422</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>23</v>
@@ -1560,21 +1547,18 @@
         <v>200</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>23</v>
@@ -1582,16 +1566,19 @@
       <c r="G11" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>23</v>
@@ -1599,16 +1586,19 @@
       <c r="G12" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H12" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>23</v>
@@ -1616,16 +1606,19 @@
       <c r="G13" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H13" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>23</v>
@@ -1633,16 +1626,19 @@
       <c r="G14" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H14" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>23</v>
@@ -1650,16 +1646,19 @@
       <c r="G15" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H15" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>23</v>
@@ -1667,16 +1666,19 @@
       <c r="G16" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H16" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>23</v>
@@ -1684,16 +1686,19 @@
       <c r="G17" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H17" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>23</v>
@@ -1701,16 +1706,19 @@
       <c r="G18" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H18" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>23</v>
@@ -1718,105 +1726,108 @@
       <c r="G19" s="19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40" t="s">
+    <row r="21" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
+    <row r="22" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
+    <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
+    <row r="24" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="16" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
+    <row r="25" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>23</v>
@@ -1828,43 +1839,48 @@
         <v>204</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>23</v>
@@ -1876,21 +1892,21 @@
         <v>204</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>23</v>
@@ -1899,64 +1915,64 @@
         <v>201</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>38</v>
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
+    <row r="33" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>38</v>
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="40" t="s">
+    <row r="35" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
       <c r="D35" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>32</v>
@@ -1964,14 +1980,14 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="16" t="s">
         <v>41</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>23</v>
@@ -1980,21 +1996,18 @@
         <v>201</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I36" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>23</v>
@@ -2003,13 +2016,10 @@
         <v>201</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I37" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -2031,82 +2041,94 @@
         <v>204</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="40" t="s">
+    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="16" t="s">
         <v>46</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G41" s="12"/>
-    </row>
-    <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
+      <c r="H41" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="16" t="s">
         <v>47</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G42" s="12"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H42" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="40" t="s">
+    <row r="44" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="40"/>
+      <c r="C44" s="39"/>
       <c r="D44" s="16" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
+      <c r="H44" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>28</v>
@@ -2114,14 +2136,14 @@
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
       <c r="D46" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>23</v>
@@ -2133,21 +2155,21 @@
         <v>204</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
       <c r="D47" s="16" t="s">
         <v>54</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F47" s="11" t="s">
         <v>23</v>
@@ -2156,24 +2178,24 @@
         <v>201</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="40"/>
-      <c r="B48" s="40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="39"/>
+      <c r="B48" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="40"/>
+      <c r="C48" s="39"/>
       <c r="D48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2182,10 +2204,10 @@
       </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="40"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
+    <row r="49" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
       <c r="D49" s="16" t="s">
         <v>57</v>
       </c>
@@ -2195,16 +2217,16 @@
       <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="40"/>
-      <c r="B50" s="40" t="s">
+      <c r="A50" s="39"/>
+      <c r="B50" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="40"/>
+      <c r="C50" s="39"/>
       <c r="D50" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>23</v>
@@ -2212,16 +2234,19 @@
       <c r="G50" s="21" t="s">
         <v>202</v>
       </c>
+      <c r="H50" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="40"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>23</v>
@@ -2231,16 +2256,16 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="40"/>
-      <c r="B52" s="40" t="s">
+      <c r="A52" s="39"/>
+      <c r="B52" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="40"/>
+      <c r="C52" s="39"/>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>23</v>
@@ -2252,21 +2277,21 @@
         <v>204</v>
       </c>
       <c r="J52" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K52" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="40"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
       <c r="D53" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>23</v>
@@ -2275,20 +2300,20 @@
         <v>201</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J53" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K53" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="K53" s="5" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="54" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="40"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
@@ -2301,9 +2326,12 @@
       <c r="G54" s="21" t="s">
         <v>202</v>
       </c>
+      <c r="H54" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="40"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
@@ -2316,20 +2344,23 @@
       <c r="G55" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="H55" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="40"/>
-      <c r="B56" s="40" t="s">
+      <c r="A56" s="39"/>
+      <c r="B56" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="39" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>69</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>23</v>
@@ -2339,14 +2370,14 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="40"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
       <c r="D57" s="16" t="s">
         <v>70</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>23</v>
@@ -2356,14 +2387,14 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="40"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
       <c r="D58" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>23</v>
@@ -2373,14 +2404,14 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="40"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
       <c r="D59" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>23</v>
@@ -2390,14 +2421,14 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
       <c r="D60" s="16" t="s">
         <v>75</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>23</v>
@@ -2406,94 +2437,94 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40" t="s">
+    <row r="61" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="39"/>
+      <c r="B61" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="40"/>
+      <c r="C61" s="39"/>
       <c r="D61" s="16" t="s">
         <v>77</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="40"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
+    <row r="62" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
       <c r="D62" s="16" t="s">
         <v>78</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
+    <row r="63" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
       <c r="D63" s="16" t="s">
         <v>79</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="40"/>
-      <c r="B64" s="40" t="s">
+    <row r="64" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="39"/>
+      <c r="B64" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="40"/>
+      <c r="C64" s="39"/>
       <c r="D64" s="16" t="s">
         <v>81</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="40"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
+    <row r="65" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="39"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
       <c r="D65" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G65" s="12"/>
     </row>
-    <row r="66" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="40"/>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
+    <row r="66" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="39"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
       <c r="D66" s="16" t="s">
         <v>83</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>28</v>
@@ -2501,14 +2532,14 @@
       <c r="G66" s="12"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="40"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
       <c r="D67" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>23</v>
@@ -2520,16 +2551,16 @@
         <v>204</v>
       </c>
       <c r="J67" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
       <c r="D68" s="16" t="s">
         <v>85</v>
       </c>
@@ -2543,21 +2574,21 @@
         <v>204</v>
       </c>
       <c r="J68" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="40"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="40"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
       <c r="D69" s="16" t="s">
         <v>86</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>23</v>
@@ -2569,21 +2600,21 @@
         <v>204</v>
       </c>
       <c r="J69" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="40"/>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
       <c r="D70" s="16" t="s">
         <v>87</v>
       </c>
       <c r="E70" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F70" s="11" t="s">
         <v>23</v>
@@ -2595,21 +2626,21 @@
         <v>204</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="40"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
+      <c r="A71" s="39"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
       <c r="D71" s="16" t="s">
         <v>88</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F71" s="11" t="s">
         <v>23</v>
@@ -2621,21 +2652,21 @@
         <v>204</v>
       </c>
       <c r="J71" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="40"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
       <c r="D72" s="16" t="s">
         <v>89</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F72" s="11" t="s">
         <v>23</v>
@@ -2647,21 +2678,21 @@
         <v>204</v>
       </c>
       <c r="J72" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
       <c r="D73" s="16" t="s">
         <v>90</v>
       </c>
       <c r="E73" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F73" s="11" t="s">
         <v>23</v>
@@ -2670,27 +2701,27 @@
         <v>201</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J73" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="40"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
       <c r="D74" s="16" t="s">
         <v>91</v>
       </c>
       <c r="E74" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F74" s="11" t="s">
         <v>23</v>
@@ -2699,27 +2730,27 @@
         <v>201</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J74" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
+      <c r="A75" s="39"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
       <c r="D75" s="33" t="s">
         <v>92</v>
       </c>
       <c r="E75" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F75" s="35" t="s">
         <v>23</v>
@@ -2728,23 +2759,23 @@
         <v>201</v>
       </c>
       <c r="H75" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I75" s="36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J75" s="37"/>
       <c r="K75" s="36"/>
     </row>
     <row r="76" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="40"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
+      <c r="A76" s="39"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
       <c r="D76" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>23</v>
@@ -2756,21 +2787,21 @@
         <v>204</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="40"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
       <c r="D77" s="16" t="s">
         <v>94</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>23</v>
@@ -2779,21 +2810,21 @@
         <v>201</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="40"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
       <c r="D78" s="16" t="s">
         <v>95</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>23</v>
@@ -2805,21 +2836,21 @@
         <v>204</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="40"/>
-      <c r="B79" s="40"/>
-      <c r="C79" s="40"/>
+      <c r="A79" s="39"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
       <c r="D79" s="24" t="s">
         <v>96</v>
       </c>
       <c r="E79" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>23</v>
@@ -2831,21 +2862,21 @@
         <v>204</v>
       </c>
       <c r="J79" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="40"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
       <c r="D80" s="24" t="s">
         <v>97</v>
       </c>
       <c r="E80" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>23</v>
@@ -2854,21 +2885,21 @@
         <v>201</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="40"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="40"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="39"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
       <c r="D81" s="16" t="s">
         <v>98</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F81" s="13" t="s">
         <v>32</v>
@@ -2876,14 +2907,14 @@
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="40"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="40"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
       <c r="D82" s="24" t="s">
         <v>99</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>23</v>
@@ -2892,27 +2923,27 @@
         <v>201</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J82" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="40"/>
-      <c r="B83" s="40"/>
-      <c r="C83" s="40"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
       <c r="D83" s="24" t="s">
         <v>100</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F83" s="11" t="s">
         <v>23</v>
@@ -2921,27 +2952,27 @@
         <v>201</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="40"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="40"/>
+      <c r="A84" s="39"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
       <c r="D84" s="24" t="s">
         <v>101</v>
       </c>
       <c r="E84" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F84" s="11" t="s">
         <v>23</v>
@@ -2950,27 +2981,27 @@
         <v>201</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J84" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="40"/>
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
+      <c r="A85" s="39"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
       <c r="D85" s="24" t="s">
         <v>102</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F85" s="11" t="s">
         <v>23</v>
@@ -2979,27 +3010,27 @@
         <v>201</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J85" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="40"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
       <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
       <c r="E86" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F86" s="11" t="s">
         <v>23</v>
@@ -3008,117 +3039,117 @@
         <v>201</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J86" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="40"/>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="39"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
       <c r="D87" s="16" t="s">
         <v>104</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F87" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="40"/>
-      <c r="B88" s="40"/>
-      <c r="C88" s="40"/>
+    <row r="88" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="39"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
       <c r="D88" s="16" t="s">
         <v>105</v>
       </c>
       <c r="E88" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F88" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="40"/>
-      <c r="B89" s="40"/>
-      <c r="C89" s="40"/>
+    <row r="89" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="39"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
       <c r="D89" s="16" t="s">
         <v>106</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F89" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="40"/>
-      <c r="B90" s="40"/>
-      <c r="C90" s="40"/>
+    <row r="90" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="39"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
       <c r="D90" s="16" t="s">
         <v>107</v>
       </c>
       <c r="E90" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F90" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="40"/>
-      <c r="B91" s="40"/>
-      <c r="C91" s="40"/>
+    <row r="91" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="39"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
       <c r="D91" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F91" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="40"/>
-      <c r="B92" s="40"/>
-      <c r="C92" s="40"/>
+    <row r="92" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="39"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
       <c r="D92" s="16" t="s">
         <v>109</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F92" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="40"/>
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
+    <row r="93" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="39"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
       <c r="D93" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F93" s="13" t="s">
         <v>32</v>
@@ -3126,14 +3157,14 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="40"/>
-      <c r="B94" s="40"/>
-      <c r="C94" s="40"/>
+      <c r="A94" s="39"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
       <c r="D94" s="24" t="s">
         <v>111</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>23</v>
@@ -3145,21 +3176,21 @@
         <v>204</v>
       </c>
       <c r="J94" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="40"/>
-      <c r="B95" s="40"/>
-      <c r="C95" s="40"/>
+      <c r="A95" s="39"/>
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
       <c r="D95" s="24" t="s">
         <v>112</v>
       </c>
       <c r="E95" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F95" s="11" t="s">
         <v>23</v>
@@ -3171,36 +3202,36 @@
         <v>204</v>
       </c>
       <c r="J95" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="40"/>
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="39"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
       <c r="D96" s="16" t="s">
         <v>113</v>
       </c>
       <c r="E96" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="40"/>
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
+    <row r="97" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="39"/>
+      <c r="B97" s="39"/>
+      <c r="C97" s="39"/>
       <c r="D97" s="16" t="s">
         <v>114</v>
       </c>
       <c r="E97" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>28</v>
@@ -3208,14 +3239,14 @@
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="40"/>
-      <c r="B98" s="40"/>
-      <c r="C98" s="40"/>
+      <c r="A98" s="39"/>
+      <c r="B98" s="39"/>
+      <c r="C98" s="39"/>
       <c r="D98" s="24" t="s">
         <v>115</v>
       </c>
       <c r="E98" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F98" s="11" t="s">
         <v>23</v>
@@ -3227,28 +3258,28 @@
         <v>204</v>
       </c>
       <c r="J98" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="38" t="s">
+      <c r="A100" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="40"/>
       <c r="D100" s="16" t="s">
         <v>117</v>
       </c>
       <c r="E100" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F100" s="11" t="s">
         <v>23</v>
@@ -3257,21 +3288,21 @@
         <v>202</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="38"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="38"/>
+      <c r="A101" s="40"/>
+      <c r="B101" s="40"/>
+      <c r="C101" s="40"/>
       <c r="D101" s="16" t="s">
         <v>118</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F101" s="11" t="s">
         <v>23</v>
@@ -3280,21 +3311,21 @@
         <v>202</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="38"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
+      <c r="A102" s="40"/>
+      <c r="B102" s="40"/>
+      <c r="C102" s="40"/>
       <c r="D102" s="16" t="s">
         <v>119</v>
       </c>
       <c r="E102" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F102" s="11" t="s">
         <v>23</v>
@@ -3307,14 +3338,14 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" s="38"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
+      <c r="A103" s="40"/>
+      <c r="B103" s="40"/>
+      <c r="C103" s="40"/>
       <c r="D103" s="16" t="s">
         <v>120</v>
       </c>
       <c r="E103" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F103" s="11" t="s">
         <v>23</v>
@@ -3326,150 +3357,150 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="40"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
+    <row r="104" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="39"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="40"/>
       <c r="D104" s="16" t="s">
         <v>121</v>
       </c>
       <c r="E104" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="40"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="38"/>
+    <row r="105" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="39"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="40"/>
       <c r="D105" s="16" t="s">
         <v>122</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="40"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="38"/>
+    <row r="106" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="39"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="40"/>
       <c r="D106" s="16" t="s">
         <v>123</v>
       </c>
       <c r="E106" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F106" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="40"/>
-      <c r="B107" s="38"/>
-      <c r="C107" s="38"/>
+    <row r="107" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="39"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="40"/>
       <c r="D107" s="16" t="s">
         <v>124</v>
       </c>
       <c r="E107" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="40"/>
-      <c r="B108" s="38"/>
-      <c r="C108" s="38"/>
+    <row r="108" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="39"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="40"/>
       <c r="D108" s="16" t="s">
         <v>125</v>
       </c>
       <c r="E108" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="40"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38"/>
+    <row r="109" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="39"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
       <c r="D109" s="16" t="s">
         <v>126</v>
       </c>
       <c r="E109" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F109" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="40"/>
-      <c r="B110" s="38"/>
-      <c r="C110" s="38"/>
+    <row r="110" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="39"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="40"/>
       <c r="D110" s="16" t="s">
         <v>127</v>
       </c>
       <c r="E110" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F110" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="40"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="38"/>
+    <row r="111" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="39"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="40"/>
       <c r="D111" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E111" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F111" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="40"/>
-      <c r="B112" s="38"/>
-      <c r="C112" s="38"/>
+    <row r="112" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="39"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="40"/>
       <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
       <c r="E112" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F112" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="40"/>
-      <c r="B113" s="38"/>
-      <c r="C113" s="38"/>
+    <row r="113" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="39"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="40"/>
       <c r="D113" s="16" t="s">
         <v>130</v>
       </c>
       <c r="E113" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F113" s="13" t="s">
         <v>32</v>
@@ -3477,14 +3508,14 @@
       <c r="G113" s="13"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" s="38"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="38"/>
+      <c r="A114" s="40"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="40"/>
       <c r="D114" s="16" t="s">
         <v>131</v>
       </c>
       <c r="E114" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F114" s="11" t="s">
         <v>23</v>
@@ -3497,14 +3528,14 @@
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" s="38"/>
-      <c r="B115" s="38"/>
-      <c r="C115" s="38"/>
+      <c r="A115" s="40"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="40"/>
       <c r="D115" s="16" t="s">
         <v>132</v>
       </c>
       <c r="E115" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F115" s="11" t="s">
         <v>23</v>
@@ -3516,57 +3547,57 @@
         <v>204</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
     </row>
-    <row r="117" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="38" t="s">
+    <row r="117" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="B117" s="38"/>
-      <c r="C117" s="38"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="40"/>
       <c r="D117" s="16" t="s">
         <v>134</v>
       </c>
       <c r="E117" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G117" s="12"/>
     </row>
-    <row r="118" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="38"/>
-      <c r="B118" s="38"/>
-      <c r="C118" s="38"/>
+    <row r="118" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="40"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="40"/>
       <c r="D118" s="16" t="s">
         <v>135</v>
       </c>
       <c r="E118" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="40" t="s">
+      <c r="A120" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="B120" s="38" t="s">
+      <c r="B120" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C120" s="38"/>
+      <c r="C120" s="40"/>
       <c r="D120" s="16" t="s">
         <v>138</v>
       </c>
       <c r="E120" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F120" s="11" t="s">
         <v>23</v>
@@ -3576,14 +3607,14 @@
       </c>
     </row>
     <row r="121" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="40"/>
-      <c r="B121" s="38"/>
-      <c r="C121" s="38"/>
+      <c r="A121" s="39"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
       <c r="D121" s="16" t="s">
         <v>139</v>
       </c>
       <c r="E121" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F121" s="11" t="s">
         <v>23</v>
@@ -3593,14 +3624,14 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="40"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="38"/>
+      <c r="A122" s="39"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
       <c r="D122" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E122" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F122" s="11" t="s">
         <v>23</v>
@@ -3610,14 +3641,14 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="40"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="38"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
       <c r="D123" s="16" t="s">
         <v>141</v>
       </c>
       <c r="E123" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F123" s="11" t="s">
         <v>23</v>
@@ -3627,14 +3658,14 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="40"/>
-      <c r="B124" s="38"/>
-      <c r="C124" s="38"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
       <c r="D124" s="24" t="s">
         <v>142</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F124" s="11" t="s">
         <v>23</v>
@@ -3643,24 +3674,24 @@
         <v>201</v>
       </c>
       <c r="I124" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J124" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K124" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="K124" s="5" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="125" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="40"/>
-      <c r="B125" s="38"/>
-      <c r="C125" s="38"/>
+      <c r="A125" s="39"/>
+      <c r="B125" s="40"/>
+      <c r="C125" s="40"/>
       <c r="D125" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E125" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F125" s="11" t="s">
         <v>23</v>
@@ -3669,18 +3700,18 @@
         <v>201</v>
       </c>
       <c r="I125" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="40"/>
-      <c r="B126" s="38"/>
-      <c r="C126" s="38"/>
+      <c r="A126" s="39"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
       <c r="D126" s="24" t="s">
         <v>144</v>
       </c>
       <c r="E126" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F126" s="11" t="s">
         <v>23</v>
@@ -3689,18 +3720,18 @@
         <v>201</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="40"/>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="40"/>
+      <c r="C127" s="40"/>
       <c r="D127" s="24" t="s">
         <v>145</v>
       </c>
       <c r="E127" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F127" s="11" t="s">
         <v>23</v>
@@ -3709,18 +3740,18 @@
         <v>201</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="40"/>
-      <c r="B128" s="38"/>
-      <c r="C128" s="38"/>
+      <c r="A128" s="39"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="40"/>
       <c r="D128" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E128" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F128" s="11" t="s">
         <v>23</v>
@@ -3729,18 +3760,18 @@
         <v>201</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="40"/>
-      <c r="B129" s="38"/>
-      <c r="C129" s="38"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="40"/>
+      <c r="C129" s="40"/>
       <c r="D129" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E129" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F129" s="11" t="s">
         <v>23</v>
@@ -3749,18 +3780,18 @@
         <v>201</v>
       </c>
       <c r="I129" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="40"/>
-      <c r="B130" s="38"/>
-      <c r="C130" s="38"/>
+      <c r="A130" s="39"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="40"/>
       <c r="D130" s="24" t="s">
         <v>148</v>
       </c>
       <c r="E130" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F130" s="11" t="s">
         <v>23</v>
@@ -3769,18 +3800,18 @@
         <v>201</v>
       </c>
       <c r="I130" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="40"/>
-      <c r="B131" s="38"/>
-      <c r="C131" s="38"/>
+      <c r="A131" s="39"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="40"/>
       <c r="D131" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E131" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>23</v>
@@ -3789,18 +3820,18 @@
         <v>201</v>
       </c>
       <c r="I131" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="40"/>
-      <c r="B132" s="38"/>
-      <c r="C132" s="38"/>
+      <c r="A132" s="39"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="40"/>
       <c r="D132" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E132" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>23</v>
@@ -3809,18 +3840,18 @@
         <v>201</v>
       </c>
       <c r="I132" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="40"/>
-      <c r="B133" s="38"/>
-      <c r="C133" s="38"/>
+      <c r="A133" s="39"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="40"/>
       <c r="D133" s="24" t="s">
         <v>151</v>
       </c>
       <c r="E133" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F133" s="11" t="s">
         <v>23</v>
@@ -3829,18 +3860,18 @@
         <v>201</v>
       </c>
       <c r="I133" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="40"/>
-      <c r="B134" s="38"/>
-      <c r="C134" s="38"/>
+      <c r="A134" s="39"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="40"/>
       <c r="D134" s="24" t="s">
         <v>152</v>
       </c>
       <c r="E134" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F134" s="11" t="s">
         <v>23</v>
@@ -3849,18 +3880,18 @@
         <v>201</v>
       </c>
       <c r="I134" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="40"/>
-      <c r="B135" s="38"/>
-      <c r="C135" s="38"/>
+      <c r="A135" s="39"/>
+      <c r="B135" s="40"/>
+      <c r="C135" s="40"/>
       <c r="D135" s="24" t="s">
         <v>153</v>
       </c>
       <c r="E135" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F135" s="11" t="s">
         <v>23</v>
@@ -3869,18 +3900,18 @@
         <v>201</v>
       </c>
       <c r="I135" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="40"/>
-      <c r="B136" s="38"/>
-      <c r="C136" s="38"/>
+      <c r="A136" s="39"/>
+      <c r="B136" s="40"/>
+      <c r="C136" s="40"/>
       <c r="D136" s="24" t="s">
         <v>154</v>
       </c>
       <c r="E136" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F136" s="11" t="s">
         <v>23</v>
@@ -3889,18 +3920,18 @@
         <v>201</v>
       </c>
       <c r="I136" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="40"/>
-      <c r="B137" s="38"/>
-      <c r="C137" s="38"/>
+      <c r="A137" s="39"/>
+      <c r="B137" s="40"/>
+      <c r="C137" s="40"/>
       <c r="D137" s="24" t="s">
         <v>155</v>
       </c>
       <c r="E137" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F137" s="11" t="s">
         <v>23</v>
@@ -3909,18 +3940,18 @@
         <v>201</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="40"/>
-      <c r="B138" s="38"/>
-      <c r="C138" s="38"/>
+      <c r="A138" s="39"/>
+      <c r="B138" s="40"/>
+      <c r="C138" s="40"/>
       <c r="D138" s="24" t="s">
         <v>156</v>
       </c>
       <c r="E138" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F138" s="11" t="s">
         <v>23</v>
@@ -3929,122 +3960,122 @@
         <v>201</v>
       </c>
       <c r="I138" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="40"/>
-      <c r="B139" s="38"/>
-      <c r="C139" s="38"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="39"/>
+      <c r="B139" s="40"/>
+      <c r="C139" s="40"/>
       <c r="D139" s="16" t="s">
         <v>157</v>
       </c>
       <c r="E139" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F139" s="15" t="s">
         <v>164</v>
       </c>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="40"/>
-      <c r="B140" s="38"/>
-      <c r="C140" s="38"/>
+    <row r="140" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="39"/>
+      <c r="B140" s="40"/>
+      <c r="C140" s="40"/>
       <c r="D140" s="16" t="s">
         <v>158</v>
       </c>
       <c r="E140" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F140" s="15" t="s">
         <v>164</v>
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
     </row>
-    <row r="142" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="38" t="s">
+    <row r="142" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="B142" s="38"/>
-      <c r="C142" s="38"/>
+      <c r="B142" s="40"/>
+      <c r="C142" s="40"/>
       <c r="D142" s="16" t="s">
         <v>160</v>
       </c>
       <c r="E142" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F142" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G142" s="12"/>
     </row>
-    <row r="143" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="38"/>
-      <c r="B143" s="38"/>
-      <c r="C143" s="38"/>
+    <row r="143" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="40"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="40"/>
       <c r="D143" s="16" t="s">
         <v>160</v>
       </c>
       <c r="E143" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F143" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G143" s="12"/>
     </row>
-    <row r="144" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="38"/>
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
+    <row r="144" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="40"/>
+      <c r="B144" s="40"/>
+      <c r="C144" s="40"/>
       <c r="D144" s="16" t="s">
         <v>161</v>
       </c>
       <c r="E144" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F144" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G144" s="12"/>
     </row>
-    <row r="145" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="38"/>
-      <c r="B145" s="38"/>
-      <c r="C145" s="38"/>
+    <row r="145" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="40"/>
+      <c r="B145" s="40"/>
+      <c r="C145" s="40"/>
       <c r="D145" s="16" t="s">
         <v>162</v>
       </c>
       <c r="E145" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F145" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G145" s="13"/>
     </row>
-    <row r="146" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="38"/>
-      <c r="B146" s="38"/>
-      <c r="C146" s="38"/>
+    <row r="146" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="40"/>
+      <c r="B146" s="40"/>
+      <c r="C146" s="40"/>
       <c r="D146" s="16" t="s">
         <v>163</v>
       </c>
       <c r="E146" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F146" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G146" s="13"/>
     </row>
-    <row r="147" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
     </row>
     <row r="148" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4061,20 +4092,20 @@
         <v>202</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
     </row>
     <row r="150" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="38" t="s">
+      <c r="A150" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="B150" s="38"/>
-      <c r="C150" s="38"/>
+      <c r="B150" s="40"/>
+      <c r="C150" s="40"/>
       <c r="D150" s="16" t="s">
         <v>168</v>
       </c>
       <c r="E150" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F150" s="11" t="s">
         <v>23</v>
@@ -4084,14 +4115,14 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="38"/>
-      <c r="B151" s="38"/>
-      <c r="C151" s="38"/>
+      <c r="A151" s="40"/>
+      <c r="B151" s="40"/>
+      <c r="C151" s="40"/>
       <c r="D151" s="16" t="s">
         <v>169</v>
       </c>
       <c r="E151" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F151" s="11" t="s">
         <v>23</v>
@@ -4100,70 +4131,70 @@
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
     </row>
-    <row r="153" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="38" t="s">
+    <row r="153" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="39"/>
-      <c r="C153" s="39"/>
+      <c r="B153" s="41"/>
+      <c r="C153" s="41"/>
       <c r="D153" s="18" t="s">
         <v>171</v>
       </c>
       <c r="E153" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G153" s="2"/>
     </row>
-    <row r="154" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="38"/>
-      <c r="B154" s="39"/>
-      <c r="C154" s="39"/>
+    <row r="154" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="40"/>
+      <c r="B154" s="41"/>
+      <c r="C154" s="41"/>
       <c r="D154" s="18" t="s">
         <v>172</v>
       </c>
       <c r="E154" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G154" s="2"/>
     </row>
-    <row r="155" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="38"/>
-      <c r="B155" s="39"/>
-      <c r="C155" s="39"/>
+    <row r="155" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="40"/>
+      <c r="B155" s="41"/>
+      <c r="C155" s="41"/>
       <c r="D155" s="18" t="s">
         <v>173</v>
       </c>
       <c r="E155" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
     </row>
     <row r="157" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="B157" s="39"/>
-      <c r="C157" s="39"/>
+      <c r="A157" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B157" s="41"/>
+      <c r="C157" s="41"/>
       <c r="D157" s="18" t="s">
         <v>174</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>23</v>
@@ -4173,14 +4204,14 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="38"/>
-      <c r="B158" s="39"/>
-      <c r="C158" s="39"/>
+      <c r="A158" s="40"/>
+      <c r="B158" s="41"/>
+      <c r="C158" s="41"/>
       <c r="D158" s="18" t="s">
         <v>175</v>
       </c>
       <c r="E158" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>23</v>
@@ -4190,14 +4221,14 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="38"/>
-      <c r="B159" s="39"/>
-      <c r="C159" s="39"/>
+      <c r="A159" s="40"/>
+      <c r="B159" s="41"/>
+      <c r="C159" s="41"/>
       <c r="D159" s="18" t="s">
         <v>176</v>
       </c>
       <c r="E159" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>23</v>
@@ -4206,57 +4237,57 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
     </row>
-    <row r="161" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="38" t="s">
+    <row r="161" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="B161" s="39"/>
-      <c r="C161" s="39"/>
+      <c r="B161" s="41"/>
+      <c r="C161" s="41"/>
       <c r="D161" s="18" t="s">
         <v>178</v>
       </c>
       <c r="E161" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="38"/>
-      <c r="B162" s="39"/>
-      <c r="C162" s="39"/>
+    <row r="162" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="40"/>
+      <c r="B162" s="41"/>
+      <c r="C162" s="41"/>
       <c r="D162" s="18" t="s">
         <v>179</v>
       </c>
       <c r="E162" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G162" s="2"/>
     </row>
-    <row r="163" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="38"/>
-      <c r="B163" s="39"/>
-      <c r="C163" s="39"/>
+    <row r="163" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="40"/>
+      <c r="B163" s="41"/>
+      <c r="C163" s="41"/>
       <c r="D163" s="18" t="s">
         <v>180</v>
       </c>
       <c r="E163" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
     </row>
     <row r="165" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4269,7 +4300,7 @@
         <v>181</v>
       </c>
       <c r="E165" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>23</v>
@@ -4278,20 +4309,20 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
     </row>
     <row r="167" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="38" t="s">
+      <c r="A167" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B167" s="39"/>
-      <c r="C167" s="39"/>
+      <c r="B167" s="41"/>
+      <c r="C167" s="41"/>
       <c r="D167" s="18" t="s">
         <v>182</v>
       </c>
       <c r="E167" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>23</v>
@@ -4301,14 +4332,14 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="38"/>
-      <c r="B168" s="39"/>
-      <c r="C168" s="39"/>
+      <c r="A168" s="40"/>
+      <c r="B168" s="41"/>
+      <c r="C168" s="41"/>
       <c r="D168" s="18" t="s">
         <v>183</v>
       </c>
       <c r="E168" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>23</v>
@@ -4317,20 +4348,20 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
     </row>
     <row r="170" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="38" t="s">
+      <c r="A170" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="B170" s="39"/>
-      <c r="C170" s="39"/>
+      <c r="B170" s="41"/>
+      <c r="C170" s="41"/>
       <c r="D170" s="18" t="s">
         <v>185</v>
       </c>
       <c r="E170" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>23</v>
@@ -4340,14 +4371,14 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="38"/>
-      <c r="B171" s="39"/>
-      <c r="C171" s="39"/>
+      <c r="A171" s="40"/>
+      <c r="B171" s="41"/>
+      <c r="C171" s="41"/>
       <c r="D171" s="18" t="s">
         <v>186</v>
       </c>
       <c r="E171" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>23</v>
@@ -4356,90 +4387,90 @@
         <v>200</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="38"/>
-      <c r="B172" s="39"/>
-      <c r="C172" s="39"/>
+    <row r="172" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="40"/>
+      <c r="B172" s="41"/>
+      <c r="C172" s="41"/>
       <c r="D172" s="18" t="s">
         <v>187</v>
       </c>
       <c r="E172" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F172" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G172" s="3"/>
     </row>
-    <row r="173" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="38"/>
-      <c r="B173" s="39"/>
-      <c r="C173" s="39"/>
+    <row r="173" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="40"/>
+      <c r="B173" s="41"/>
+      <c r="C173" s="41"/>
       <c r="D173" s="18" t="s">
         <v>188</v>
       </c>
       <c r="E173" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F173" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
     </row>
-    <row r="175" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="38" t="s">
+    <row r="175" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="38"/>
-      <c r="C175" s="38"/>
+      <c r="B175" s="40"/>
+      <c r="C175" s="40"/>
       <c r="D175" s="18" t="s">
         <v>190</v>
       </c>
       <c r="E175" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G175" s="2"/>
     </row>
-    <row r="176" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="38"/>
-      <c r="B176" s="38"/>
-      <c r="C176" s="38"/>
+    <row r="176" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="40"/>
+      <c r="B176" s="40"/>
+      <c r="C176" s="40"/>
       <c r="D176" s="18" t="s">
         <v>191</v>
       </c>
       <c r="E176" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F176" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="38"/>
-      <c r="B177" s="38"/>
-      <c r="C177" s="38"/>
+    <row r="177" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="40"/>
+      <c r="B177" s="40"/>
+      <c r="C177" s="40"/>
       <c r="D177" s="18" t="s">
         <v>192</v>
       </c>
       <c r="E177" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F177" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
     </row>
-    <row r="179" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>193</v>
       </c>
@@ -4449,14 +4480,14 @@
         <v>194</v>
       </c>
       <c r="E179" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G179" s="2"/>
     </row>
-    <row r="180" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
     </row>
     <row r="181" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4472,10 +4503,10 @@
         <v>200</v>
       </c>
       <c r="H181" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I181" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4511,14 +4542,64 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:H183" xr:uid="{9EEAC858-8201-E147-9707-1E1D2225B431}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="GET"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="E1:H183" xr:uid="{9EEAC858-8201-E147-9707-1E1D2225B431}"/>
   <mergeCells count="72">
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C140"/>
+    <mergeCell ref="B124:B140"/>
+    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A100:A115"/>
+    <mergeCell ref="B100:B115"/>
+    <mergeCell ref="C100:C115"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C5:C19"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="L1:L1048576"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="B41:B42"/>
@@ -4535,62 +4616,6 @@
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C5:C19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A100:A115"/>
-    <mergeCell ref="B100:B115"/>
-    <mergeCell ref="C100:C115"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C140"/>
-    <mergeCell ref="B124:B140"/>
-    <mergeCell ref="A120:A140"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="C170:C173"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update collection and environment files
</commit_message>
<xml_diff>
--- a/Census_Wsc_Services.xlsx
+++ b/Census_Wsc_Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463140B-7920-F644-AFA9-AC5E8AD46BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E740F-5F53-414D-BE77-D01BCCD3FEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>

</xml_diff>